<commit_message>
Code & updated Plannung
</commit_message>
<xml_diff>
--- a/docs/Zeitplanung.xlsx
+++ b/docs/Zeitplanung.xlsx
@@ -5,13 +5,13 @@
   <workbookPr codeName="DieseArbeitsmappe" showPivotChartFilter="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sluz-my.sharepoint.com/personal/natascha_mueller1_sluz_ch/Documents/Basislehrjahr/Memory collector/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/natascha/Desktop/Memory-Collector/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="123" documentId="8_{449300B2-FE85-C544-9688-0071A5260D40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CE2D963A-9074-A642-A563-B1036CF23105}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39061389-E65D-234E-8B3C-39884144E51F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="35840" yWindow="-9280" windowWidth="38400" windowHeight="21600" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35840" yWindow="-8820" windowWidth="38400" windowHeight="21140" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zeitplanung" sheetId="1" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="61">
   <si>
     <t>Nr.</t>
   </si>
@@ -229,18 +229,6 @@
     <t>Project Abstract erstellen</t>
   </si>
   <si>
-    <t>Texte Hinzufügen</t>
-  </si>
-  <si>
-    <t>Datum anzeigen</t>
-  </si>
-  <si>
-    <t>Bilder hinzufügen</t>
-  </si>
-  <si>
-    <t>Beiträge nach Datum sortieren</t>
-  </si>
-  <si>
     <t>Grundlage für App</t>
   </si>
   <si>
@@ -248,6 +236,33 @@
   </si>
   <si>
     <t>Memory Collecter</t>
+  </si>
+  <si>
+    <t>A003: Erinnerung erstellen</t>
+  </si>
+  <si>
+    <t>A001: Erinnerungen anzeigen</t>
+  </si>
+  <si>
+    <t>A002: Erinnerungen Einzelansicht</t>
+  </si>
+  <si>
+    <t>A004: Titel zur Erinnerung</t>
+  </si>
+  <si>
+    <t>A005: Beschreibung der Erinnerung</t>
+  </si>
+  <si>
+    <t>A006: Bild zu Erinnerung</t>
+  </si>
+  <si>
+    <t>A007: Erstelldatum der Erinnerung</t>
+  </si>
+  <si>
+    <t>A008: Erstellort der Erinnerung</t>
+  </si>
+  <si>
+    <t>A010: Erinnerungen sortieren</t>
   </si>
 </sst>
 </file>
@@ -1111,7 +1126,7 @@
     </xf>
     <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1420,6 +1435,26 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="1" borderId="38" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1451,23 +1486,13 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="1" borderId="38" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1577,7 +1602,7 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>54.5</c:v>
+                  <c:v>60.800000000000011</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>8.5</c:v>
@@ -1645,10 +1670,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>4.16</c:v>
+                  <c:v>2.3199999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2159,7 +2184,7 @@
   <dimension ref="A1:BJ43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="R20" sqref="R20"/>
+      <selection activeCell="X35" sqref="X35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2175,7 +2200,7 @@
   <sheetData>
     <row r="1" spans="1:62" ht="25" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -2478,88 +2503,88 @@
     <row r="7" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9"/>
       <c r="B7" s="27"/>
-      <c r="C7" s="92" t="s">
+      <c r="C7" s="97" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="92"/>
+      <c r="D7" s="97"/>
       <c r="E7" s="28" t="s">
         <v>20</v>
       </c>
       <c r="F7" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="93" t="s">
+      <c r="G7" s="98" t="s">
         <v>32</v>
       </c>
-      <c r="H7" s="93"/>
-      <c r="I7" s="93"/>
-      <c r="J7" s="93"/>
-      <c r="K7" s="93"/>
-      <c r="L7" s="93"/>
-      <c r="M7" s="94"/>
-      <c r="N7" s="93" t="s">
+      <c r="H7" s="98"/>
+      <c r="I7" s="98"/>
+      <c r="J7" s="98"/>
+      <c r="K7" s="98"/>
+      <c r="L7" s="98"/>
+      <c r="M7" s="99"/>
+      <c r="N7" s="98" t="s">
         <v>33</v>
       </c>
-      <c r="O7" s="93"/>
-      <c r="P7" s="93"/>
-      <c r="Q7" s="93"/>
-      <c r="R7" s="93"/>
-      <c r="S7" s="93"/>
-      <c r="T7" s="94"/>
-      <c r="U7" s="93" t="s">
+      <c r="O7" s="98"/>
+      <c r="P7" s="98"/>
+      <c r="Q7" s="98"/>
+      <c r="R7" s="98"/>
+      <c r="S7" s="98"/>
+      <c r="T7" s="99"/>
+      <c r="U7" s="98" t="s">
         <v>34</v>
       </c>
-      <c r="V7" s="93"/>
-      <c r="W7" s="93"/>
-      <c r="X7" s="93"/>
-      <c r="Y7" s="93"/>
-      <c r="Z7" s="93"/>
-      <c r="AA7" s="94"/>
-      <c r="AB7" s="95" t="s">
+      <c r="V7" s="98"/>
+      <c r="W7" s="98"/>
+      <c r="X7" s="98"/>
+      <c r="Y7" s="98"/>
+      <c r="Z7" s="98"/>
+      <c r="AA7" s="99"/>
+      <c r="AB7" s="100" t="s">
         <v>35</v>
       </c>
-      <c r="AC7" s="93"/>
-      <c r="AD7" s="93"/>
-      <c r="AE7" s="93"/>
-      <c r="AF7" s="93"/>
-      <c r="AG7" s="93"/>
-      <c r="AH7" s="94"/>
-      <c r="AI7" s="93" t="s">
-        <v>54</v>
-      </c>
-      <c r="AJ7" s="93"/>
-      <c r="AK7" s="93"/>
-      <c r="AL7" s="93"/>
-      <c r="AM7" s="93"/>
-      <c r="AN7" s="93"/>
-      <c r="AO7" s="94"/>
-      <c r="AP7" s="95" t="s">
+      <c r="AC7" s="98"/>
+      <c r="AD7" s="98"/>
+      <c r="AE7" s="98"/>
+      <c r="AF7" s="98"/>
+      <c r="AG7" s="98"/>
+      <c r="AH7" s="99"/>
+      <c r="AI7" s="98" t="s">
+        <v>50</v>
+      </c>
+      <c r="AJ7" s="98"/>
+      <c r="AK7" s="98"/>
+      <c r="AL7" s="98"/>
+      <c r="AM7" s="98"/>
+      <c r="AN7" s="98"/>
+      <c r="AO7" s="99"/>
+      <c r="AP7" s="100" t="s">
         <v>36</v>
       </c>
-      <c r="AQ7" s="93"/>
-      <c r="AR7" s="93"/>
-      <c r="AS7" s="93"/>
-      <c r="AT7" s="93"/>
-      <c r="AU7" s="93"/>
-      <c r="AV7" s="94"/>
-      <c r="AW7" s="93" t="s">
+      <c r="AQ7" s="98"/>
+      <c r="AR7" s="98"/>
+      <c r="AS7" s="98"/>
+      <c r="AT7" s="98"/>
+      <c r="AU7" s="98"/>
+      <c r="AV7" s="99"/>
+      <c r="AW7" s="98" t="s">
         <v>37</v>
       </c>
-      <c r="AX7" s="93"/>
-      <c r="AY7" s="93"/>
-      <c r="AZ7" s="93"/>
-      <c r="BA7" s="93"/>
-      <c r="BB7" s="93"/>
-      <c r="BC7" s="94"/>
-      <c r="BD7" s="95" t="s">
+      <c r="AX7" s="98"/>
+      <c r="AY7" s="98"/>
+      <c r="AZ7" s="98"/>
+      <c r="BA7" s="98"/>
+      <c r="BB7" s="98"/>
+      <c r="BC7" s="99"/>
+      <c r="BD7" s="100" t="s">
         <v>38</v>
       </c>
-      <c r="BE7" s="93"/>
-      <c r="BF7" s="93"/>
-      <c r="BG7" s="93"/>
-      <c r="BH7" s="93"/>
-      <c r="BI7" s="93"/>
-      <c r="BJ7" s="96"/>
+      <c r="BE7" s="98"/>
+      <c r="BF7" s="98"/>
+      <c r="BG7" s="98"/>
+      <c r="BH7" s="98"/>
+      <c r="BI7" s="98"/>
+      <c r="BJ7" s="101"/>
     </row>
     <row r="8" spans="1:62" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
@@ -2760,7 +2785,7 @@
       </c>
       <c r="D9" s="42">
         <f>SUM(D10:D13)</f>
-        <v>4.16</v>
+        <v>2.3199999999999998</v>
       </c>
       <c r="E9" s="32"/>
       <c r="F9" s="31"/>
@@ -2861,9 +2886,9 @@
       <c r="AA10" s="58"/>
       <c r="AB10" s="55"/>
       <c r="AC10" s="55"/>
-      <c r="AD10" s="101"/>
-      <c r="AE10" s="101"/>
-      <c r="AF10" s="101"/>
+      <c r="AD10" s="92"/>
+      <c r="AE10" s="92"/>
+      <c r="AF10" s="92"/>
       <c r="AG10" s="57"/>
       <c r="AH10" s="58"/>
       <c r="AI10" s="53"/>
@@ -2907,7 +2932,7 @@
       </c>
       <c r="D11" s="82">
         <f>SUM(G11:BJ11)</f>
-        <v>3.84</v>
+        <v>2</v>
       </c>
       <c r="E11" s="50">
         <v>1</v>
@@ -2916,8 +2941,8 @@
       <c r="G11" s="59"/>
       <c r="H11" s="60"/>
       <c r="I11" s="61"/>
-      <c r="J11" s="102">
-        <v>3.84</v>
+      <c r="J11" s="93">
+        <v>2</v>
       </c>
       <c r="K11" s="84"/>
       <c r="L11" s="62"/>
@@ -2942,9 +2967,9 @@
       <c r="AA11" s="58"/>
       <c r="AB11" s="55"/>
       <c r="AC11" s="55"/>
-      <c r="AD11" s="101"/>
-      <c r="AE11" s="101"/>
-      <c r="AF11" s="101"/>
+      <c r="AD11" s="92"/>
+      <c r="AE11" s="92"/>
+      <c r="AF11" s="92"/>
       <c r="AG11" s="57"/>
       <c r="AH11" s="58"/>
       <c r="AI11" s="59"/>
@@ -2997,7 +3022,7 @@
       <c r="G12" s="59"/>
       <c r="H12" s="60"/>
       <c r="I12" s="61"/>
-      <c r="J12" s="104">
+      <c r="J12" s="95">
         <v>0.16</v>
       </c>
       <c r="K12" s="63">
@@ -3021,9 +3046,9 @@
       <c r="AA12" s="58"/>
       <c r="AB12" s="55"/>
       <c r="AC12" s="55"/>
-      <c r="AD12" s="101"/>
-      <c r="AE12" s="101"/>
-      <c r="AF12" s="101"/>
+      <c r="AD12" s="92"/>
+      <c r="AE12" s="92"/>
+      <c r="AF12" s="92"/>
       <c r="AG12" s="57"/>
       <c r="AH12" s="58"/>
       <c r="AI12" s="59"/>
@@ -3095,9 +3120,9 @@
       <c r="AA13" s="67"/>
       <c r="AB13" s="55"/>
       <c r="AC13" s="55"/>
-      <c r="AD13" s="101"/>
-      <c r="AE13" s="101"/>
-      <c r="AF13" s="101"/>
+      <c r="AD13" s="92"/>
+      <c r="AE13" s="92"/>
+      <c r="AF13" s="92"/>
       <c r="AG13" s="66"/>
       <c r="AH13" s="67"/>
       <c r="AI13" s="59"/>
@@ -3142,7 +3167,7 @@
       </c>
       <c r="D14" s="42">
         <f>SUM(D15:D17)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E14" s="32"/>
       <c r="F14" s="31"/>
@@ -3215,7 +3240,7 @@
       </c>
       <c r="D15" s="82">
         <f>SUM(G15:BJ15)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E15" s="50"/>
       <c r="F15" s="88" t="s">
@@ -3224,7 +3249,9 @@
       <c r="G15" s="53"/>
       <c r="H15" s="54"/>
       <c r="I15" s="55"/>
-      <c r="J15" s="55"/>
+      <c r="J15" s="94">
+        <v>4</v>
+      </c>
       <c r="K15" s="86"/>
       <c r="L15" s="57"/>
       <c r="M15" s="58"/>
@@ -3244,9 +3271,9 @@
       <c r="AA15" s="58"/>
       <c r="AB15" s="55"/>
       <c r="AC15" s="55"/>
-      <c r="AD15" s="101"/>
-      <c r="AE15" s="101"/>
-      <c r="AF15" s="101"/>
+      <c r="AD15" s="92"/>
+      <c r="AE15" s="92"/>
+      <c r="AF15" s="92"/>
       <c r="AG15" s="57"/>
       <c r="AH15" s="58"/>
       <c r="AI15" s="53"/>
@@ -3317,9 +3344,9 @@
       <c r="AA16" s="58"/>
       <c r="AB16" s="55"/>
       <c r="AC16" s="55"/>
-      <c r="AD16" s="101"/>
-      <c r="AE16" s="101"/>
-      <c r="AF16" s="101"/>
+      <c r="AD16" s="92"/>
+      <c r="AE16" s="92"/>
+      <c r="AF16" s="92"/>
       <c r="AG16" s="57"/>
       <c r="AH16" s="58"/>
       <c r="AI16" s="59"/>
@@ -3386,9 +3413,9 @@
       <c r="AA17" s="58"/>
       <c r="AB17" s="55"/>
       <c r="AC17" s="55"/>
-      <c r="AD17" s="101"/>
-      <c r="AE17" s="101"/>
-      <c r="AF17" s="101"/>
+      <c r="AD17" s="92"/>
+      <c r="AE17" s="92"/>
+      <c r="AF17" s="92"/>
       <c r="AG17" s="57"/>
       <c r="AH17" s="58"/>
       <c r="AI17" s="68"/>
@@ -3429,7 +3456,7 @@
       </c>
       <c r="C18" s="41">
         <f>SUM(C19:C30)</f>
-        <v>54.5</v>
+        <v>60.800000000000011</v>
       </c>
       <c r="D18" s="42">
         <f>SUM(D19:D30)</f>
@@ -3533,9 +3560,9 @@
       <c r="AA19" s="58"/>
       <c r="AB19" s="55"/>
       <c r="AC19" s="55"/>
-      <c r="AD19" s="101"/>
-      <c r="AE19" s="101"/>
-      <c r="AF19" s="101"/>
+      <c r="AD19" s="92"/>
+      <c r="AE19" s="92"/>
+      <c r="AF19" s="92"/>
       <c r="AG19" s="57"/>
       <c r="AH19" s="58"/>
       <c r="AI19" s="53"/>
@@ -3587,13 +3614,13 @@
       <c r="H20" s="60"/>
       <c r="I20" s="55"/>
       <c r="J20" s="55"/>
-      <c r="K20" s="105"/>
+      <c r="K20" s="96"/>
       <c r="L20" s="57"/>
       <c r="M20" s="58"/>
       <c r="N20" s="59"/>
       <c r="O20" s="60"/>
-      <c r="P20" s="103"/>
-      <c r="Q20" s="103"/>
+      <c r="P20" s="94"/>
+      <c r="Q20" s="107"/>
       <c r="R20" s="55"/>
       <c r="S20" s="57"/>
       <c r="T20" s="58"/>
@@ -3601,14 +3628,14 @@
       <c r="V20" s="60"/>
       <c r="W20" s="55"/>
       <c r="X20" s="55"/>
-      <c r="Y20" s="56"/>
+      <c r="Y20" s="55"/>
       <c r="Z20" s="57"/>
       <c r="AA20" s="58"/>
       <c r="AB20" s="55"/>
       <c r="AC20" s="55"/>
-      <c r="AD20" s="101"/>
-      <c r="AE20" s="101"/>
-      <c r="AF20" s="101"/>
+      <c r="AD20" s="92"/>
+      <c r="AE20" s="92"/>
+      <c r="AF20" s="92"/>
       <c r="AG20" s="57"/>
       <c r="AH20" s="58"/>
       <c r="AI20" s="59"/>
@@ -3645,7 +3672,7 @@
         <v>303</v>
       </c>
       <c r="B21" s="46" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C21" s="49">
         <v>5</v>
@@ -3662,28 +3689,28 @@
       <c r="H21" s="60"/>
       <c r="I21" s="55"/>
       <c r="J21" s="55"/>
-      <c r="K21" s="56"/>
+      <c r="K21" s="63"/>
       <c r="L21" s="57"/>
       <c r="M21" s="58"/>
       <c r="N21" s="59"/>
       <c r="O21" s="60"/>
-      <c r="P21" s="55"/>
+      <c r="P21" s="94"/>
       <c r="Q21" s="55"/>
       <c r="R21" s="56"/>
       <c r="S21" s="57"/>
       <c r="T21" s="58"/>
       <c r="U21" s="59"/>
       <c r="V21" s="60"/>
-      <c r="W21" s="103"/>
+      <c r="W21" s="55"/>
       <c r="X21" s="55"/>
-      <c r="Y21" s="56"/>
+      <c r="Y21" s="55"/>
       <c r="Z21" s="57"/>
       <c r="AA21" s="58"/>
       <c r="AB21" s="55"/>
       <c r="AC21" s="55"/>
-      <c r="AD21" s="101"/>
-      <c r="AE21" s="101"/>
-      <c r="AF21" s="101"/>
+      <c r="AD21" s="92"/>
+      <c r="AE21" s="92"/>
+      <c r="AF21" s="92"/>
       <c r="AG21" s="57"/>
       <c r="AH21" s="58"/>
       <c r="AI21" s="59"/>
@@ -3720,10 +3747,10 @@
         <v>304</v>
       </c>
       <c r="B22" s="46" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C22" s="49">
-        <v>3.5</v>
+        <v>2</v>
       </c>
       <c r="D22" s="82">
         <f t="shared" si="0"/>
@@ -3749,16 +3776,16 @@
       <c r="T22" s="58"/>
       <c r="U22" s="59"/>
       <c r="V22" s="60"/>
-      <c r="W22" s="55"/>
-      <c r="X22" s="103"/>
-      <c r="Y22" s="56"/>
+      <c r="W22" s="94"/>
+      <c r="X22" s="94"/>
+      <c r="Y22" s="94"/>
       <c r="Z22" s="57"/>
       <c r="AA22" s="58"/>
       <c r="AB22" s="55"/>
-      <c r="AC22" s="103"/>
-      <c r="AD22" s="101"/>
-      <c r="AE22" s="101"/>
-      <c r="AF22" s="101"/>
+      <c r="AC22" s="55"/>
+      <c r="AD22" s="92"/>
+      <c r="AE22" s="92"/>
+      <c r="AF22" s="92"/>
       <c r="AG22" s="57"/>
       <c r="AH22" s="58"/>
       <c r="AI22" s="59"/>
@@ -3795,10 +3822,10 @@
         <v>305</v>
       </c>
       <c r="B23" s="46" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C23" s="49">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D23" s="82">
         <f t="shared" si="0"/>
@@ -3824,16 +3851,16 @@
       <c r="T23" s="58"/>
       <c r="U23" s="59"/>
       <c r="V23" s="60"/>
-      <c r="W23" s="61"/>
-      <c r="X23" s="102"/>
-      <c r="Y23" s="56"/>
+      <c r="W23" s="55"/>
+      <c r="X23" s="55"/>
+      <c r="Y23" s="55"/>
       <c r="Z23" s="57"/>
       <c r="AA23" s="58"/>
       <c r="AB23" s="55"/>
-      <c r="AC23" s="103"/>
-      <c r="AD23" s="101"/>
-      <c r="AE23" s="101"/>
-      <c r="AF23" s="101"/>
+      <c r="AC23" s="55"/>
+      <c r="AD23" s="92"/>
+      <c r="AE23" s="92"/>
+      <c r="AF23" s="92"/>
       <c r="AG23" s="57"/>
       <c r="AH23" s="58"/>
       <c r="AI23" s="59"/>
@@ -3870,7 +3897,7 @@
         <v>306</v>
       </c>
       <c r="B24" s="46" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C24" s="49">
         <v>9</v>
@@ -3893,22 +3920,22 @@
       <c r="N24" s="59"/>
       <c r="O24" s="60"/>
       <c r="P24" s="55"/>
-      <c r="Q24" s="55"/>
-      <c r="R24" s="56"/>
+      <c r="Q24" s="94"/>
+      <c r="R24" s="63"/>
       <c r="S24" s="57"/>
       <c r="T24" s="58"/>
       <c r="U24" s="59"/>
       <c r="V24" s="60"/>
-      <c r="W24" s="55"/>
+      <c r="W24" s="108"/>
       <c r="X24" s="55"/>
-      <c r="Y24" s="63"/>
+      <c r="Y24" s="55"/>
       <c r="Z24" s="57"/>
       <c r="AA24" s="58"/>
-      <c r="AB24" s="103"/>
-      <c r="AC24" s="103"/>
-      <c r="AD24" s="101"/>
-      <c r="AE24" s="101"/>
-      <c r="AF24" s="101"/>
+      <c r="AB24" s="55"/>
+      <c r="AC24" s="55"/>
+      <c r="AD24" s="92"/>
+      <c r="AE24" s="92"/>
+      <c r="AF24" s="92"/>
       <c r="AG24" s="57"/>
       <c r="AH24" s="58"/>
       <c r="AI24" s="59"/>
@@ -3944,13 +3971,19 @@
       <c r="A25" s="12">
         <v>307</v>
       </c>
-      <c r="B25" s="46"/>
-      <c r="C25" s="49"/>
+      <c r="B25" s="46" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="49">
+        <v>0.7</v>
+      </c>
       <c r="D25" s="82">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E25" s="50"/>
+      <c r="E25" s="50">
+        <v>1</v>
+      </c>
       <c r="F25" s="51"/>
       <c r="G25" s="59"/>
       <c r="H25" s="60"/>
@@ -3962,7 +3995,7 @@
       <c r="N25" s="59"/>
       <c r="O25" s="60"/>
       <c r="P25" s="55"/>
-      <c r="Q25" s="55"/>
+      <c r="Q25" s="94"/>
       <c r="R25" s="56"/>
       <c r="S25" s="57"/>
       <c r="T25" s="58"/>
@@ -3970,14 +4003,14 @@
       <c r="V25" s="60"/>
       <c r="W25" s="55"/>
       <c r="X25" s="55"/>
-      <c r="Y25" s="56"/>
+      <c r="Y25" s="55"/>
       <c r="Z25" s="57"/>
       <c r="AA25" s="58"/>
       <c r="AB25" s="55"/>
       <c r="AC25" s="55"/>
-      <c r="AD25" s="101"/>
-      <c r="AE25" s="101"/>
-      <c r="AF25" s="101"/>
+      <c r="AD25" s="92"/>
+      <c r="AE25" s="92"/>
+      <c r="AF25" s="92"/>
       <c r="AG25" s="57"/>
       <c r="AH25" s="58"/>
       <c r="AI25" s="59"/>
@@ -4014,15 +4047,17 @@
         <v>308</v>
       </c>
       <c r="B26" s="46" t="s">
-        <v>52</v>
-      </c>
-      <c r="C26" s="49"/>
+        <v>56</v>
+      </c>
+      <c r="C26" s="49">
+        <v>0.7</v>
+      </c>
       <c r="D26" s="82">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E26" s="50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F26" s="51"/>
       <c r="G26" s="59"/>
@@ -4036,21 +4071,21 @@
       <c r="O26" s="60"/>
       <c r="P26" s="55"/>
       <c r="Q26" s="55"/>
-      <c r="R26" s="56"/>
+      <c r="R26" s="63"/>
       <c r="S26" s="57"/>
       <c r="T26" s="58"/>
       <c r="U26" s="59"/>
       <c r="V26" s="60"/>
       <c r="W26" s="55"/>
       <c r="X26" s="55"/>
-      <c r="Y26" s="56"/>
+      <c r="Y26" s="55"/>
       <c r="Z26" s="57"/>
       <c r="AA26" s="58"/>
       <c r="AB26" s="55"/>
       <c r="AC26" s="55"/>
-      <c r="AD26" s="101"/>
-      <c r="AE26" s="101"/>
-      <c r="AF26" s="101"/>
+      <c r="AD26" s="92"/>
+      <c r="AE26" s="92"/>
+      <c r="AF26" s="92"/>
       <c r="AG26" s="57"/>
       <c r="AH26" s="58"/>
       <c r="AI26" s="59"/>
@@ -4086,13 +4121,19 @@
       <c r="A27" s="12">
         <v>309</v>
       </c>
-      <c r="B27" s="46"/>
-      <c r="C27" s="49"/>
+      <c r="B27" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="49">
+        <v>3</v>
+      </c>
       <c r="D27" s="82">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E27" s="50"/>
+      <c r="E27" s="50">
+        <v>1</v>
+      </c>
       <c r="F27" s="51"/>
       <c r="G27" s="59"/>
       <c r="H27" s="60"/>
@@ -4110,16 +4151,16 @@
       <c r="T27" s="58"/>
       <c r="U27" s="59"/>
       <c r="V27" s="60"/>
-      <c r="W27" s="55"/>
-      <c r="X27" s="55"/>
-      <c r="Y27" s="56"/>
+      <c r="W27" s="94"/>
+      <c r="X27" s="94"/>
+      <c r="Y27" s="55"/>
       <c r="Z27" s="57"/>
       <c r="AA27" s="58"/>
       <c r="AB27" s="55"/>
       <c r="AC27" s="55"/>
-      <c r="AD27" s="101"/>
-      <c r="AE27" s="101"/>
-      <c r="AF27" s="101"/>
+      <c r="AD27" s="92"/>
+      <c r="AE27" s="92"/>
+      <c r="AF27" s="92"/>
       <c r="AG27" s="57"/>
       <c r="AH27" s="58"/>
       <c r="AI27" s="59"/>
@@ -4155,13 +4196,19 @@
       <c r="A28" s="12">
         <v>310</v>
       </c>
-      <c r="B28" s="46"/>
-      <c r="C28" s="49"/>
+      <c r="B28" s="46" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" s="49">
+        <v>0.7</v>
+      </c>
       <c r="D28" s="82">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E28" s="50"/>
+      <c r="E28" s="50">
+        <v>1</v>
+      </c>
       <c r="F28" s="51"/>
       <c r="G28" s="59"/>
       <c r="H28" s="60"/>
@@ -4179,16 +4226,16 @@
       <c r="T28" s="58"/>
       <c r="U28" s="59"/>
       <c r="V28" s="60"/>
-      <c r="W28" s="55"/>
-      <c r="X28" s="55"/>
-      <c r="Y28" s="56"/>
+      <c r="W28" s="94"/>
+      <c r="X28" s="94"/>
+      <c r="Y28" s="55"/>
       <c r="Z28" s="57"/>
       <c r="AA28" s="58"/>
       <c r="AB28" s="55"/>
       <c r="AC28" s="55"/>
-      <c r="AD28" s="101"/>
-      <c r="AE28" s="101"/>
-      <c r="AF28" s="101"/>
+      <c r="AD28" s="92"/>
+      <c r="AE28" s="92"/>
+      <c r="AF28" s="92"/>
       <c r="AG28" s="57"/>
       <c r="AH28" s="58"/>
       <c r="AI28" s="59"/>
@@ -4224,13 +4271,19 @@
       <c r="A29" s="12">
         <v>311</v>
       </c>
-      <c r="B29" s="46"/>
-      <c r="C29" s="49"/>
+      <c r="B29" s="46" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" s="49">
+        <v>0.7</v>
+      </c>
       <c r="D29" s="82">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E29" s="50"/>
+      <c r="E29" s="50">
+        <v>2</v>
+      </c>
       <c r="F29" s="51"/>
       <c r="G29" s="70"/>
       <c r="H29" s="71"/>
@@ -4248,16 +4301,16 @@
       <c r="T29" s="58"/>
       <c r="U29" s="70"/>
       <c r="V29" s="71"/>
-      <c r="W29" s="55"/>
-      <c r="X29" s="55"/>
-      <c r="Y29" s="56"/>
+      <c r="W29" s="94"/>
+      <c r="X29" s="94"/>
+      <c r="Y29" s="55"/>
       <c r="Z29" s="57"/>
       <c r="AA29" s="58"/>
       <c r="AB29" s="55"/>
       <c r="AC29" s="55"/>
-      <c r="AD29" s="101"/>
-      <c r="AE29" s="101"/>
-      <c r="AF29" s="101"/>
+      <c r="AD29" s="92"/>
+      <c r="AE29" s="92"/>
+      <c r="AF29" s="92"/>
       <c r="AG29" s="57"/>
       <c r="AH29" s="58"/>
       <c r="AI29" s="70"/>
@@ -4293,13 +4346,19 @@
       <c r="A30" s="12">
         <v>312</v>
       </c>
-      <c r="B30" s="46"/>
-      <c r="C30" s="49"/>
+      <c r="B30" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="49">
+        <v>3</v>
+      </c>
       <c r="D30" s="82">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E30" s="50"/>
+      <c r="E30" s="50">
+        <v>2</v>
+      </c>
       <c r="F30" s="51"/>
       <c r="G30" s="68"/>
       <c r="H30" s="69"/>
@@ -4319,14 +4378,14 @@
       <c r="V30" s="69"/>
       <c r="W30" s="55"/>
       <c r="X30" s="55"/>
-      <c r="Y30" s="56"/>
+      <c r="Y30" s="63"/>
       <c r="Z30" s="57"/>
       <c r="AA30" s="58"/>
-      <c r="AB30" s="55"/>
+      <c r="AB30" s="94"/>
       <c r="AC30" s="55"/>
-      <c r="AD30" s="101"/>
-      <c r="AE30" s="101"/>
-      <c r="AF30" s="101"/>
+      <c r="AD30" s="92"/>
+      <c r="AE30" s="92"/>
+      <c r="AF30" s="92"/>
       <c r="AG30" s="57"/>
       <c r="AH30" s="58"/>
       <c r="AI30" s="68"/>
@@ -4459,21 +4518,21 @@
       <c r="O32" s="54"/>
       <c r="P32" s="55"/>
       <c r="Q32" s="55"/>
-      <c r="R32" s="56"/>
+      <c r="R32" s="63"/>
       <c r="S32" s="57"/>
       <c r="T32" s="58"/>
       <c r="U32" s="53"/>
       <c r="V32" s="54"/>
       <c r="W32" s="55"/>
-      <c r="X32" s="103"/>
-      <c r="Y32" s="56"/>
-      <c r="Z32" s="57"/>
+      <c r="X32" s="55"/>
+      <c r="Y32" s="55"/>
+      <c r="Z32" s="58"/>
       <c r="AA32" s="58"/>
       <c r="AB32" s="55"/>
       <c r="AC32" s="55"/>
-      <c r="AD32" s="101"/>
-      <c r="AE32" s="101"/>
-      <c r="AF32" s="101"/>
+      <c r="AD32" s="92"/>
+      <c r="AE32" s="92"/>
+      <c r="AF32" s="92"/>
       <c r="AG32" s="57"/>
       <c r="AH32" s="58"/>
       <c r="AI32" s="53"/>
@@ -4487,7 +4546,7 @@
       <c r="AQ32" s="54"/>
       <c r="AR32" s="55"/>
       <c r="AS32" s="55"/>
-      <c r="AT32" s="56"/>
+      <c r="AT32" s="55"/>
       <c r="AU32" s="57"/>
       <c r="AV32" s="58"/>
       <c r="AW32" s="53"/>
@@ -4537,16 +4596,16 @@
       <c r="T33" s="58"/>
       <c r="U33" s="59"/>
       <c r="V33" s="60"/>
-      <c r="W33" s="55"/>
-      <c r="X33" s="55"/>
-      <c r="Y33" s="56"/>
-      <c r="Z33" s="57"/>
+      <c r="W33" s="94"/>
+      <c r="X33" s="94"/>
+      <c r="Y33" s="94"/>
+      <c r="Z33" s="58"/>
       <c r="AA33" s="58"/>
-      <c r="AB33" s="103"/>
-      <c r="AC33" s="103"/>
-      <c r="AD33" s="101"/>
-      <c r="AE33" s="101"/>
-      <c r="AF33" s="101"/>
+      <c r="AB33" s="94"/>
+      <c r="AC33" s="94"/>
+      <c r="AD33" s="92"/>
+      <c r="AE33" s="92"/>
+      <c r="AF33" s="92"/>
       <c r="AG33" s="57"/>
       <c r="AH33" s="58"/>
       <c r="AI33" s="59"/>
@@ -4558,8 +4617,8 @@
       <c r="AO33" s="58"/>
       <c r="AP33" s="59"/>
       <c r="AQ33" s="60"/>
-      <c r="AR33" s="103"/>
-      <c r="AS33" s="103"/>
+      <c r="AR33" s="55"/>
+      <c r="AS33" s="55"/>
       <c r="AT33" s="55"/>
       <c r="AU33" s="57"/>
       <c r="AV33" s="58"/>
@@ -4610,16 +4669,16 @@
       <c r="T34" s="58"/>
       <c r="U34" s="59"/>
       <c r="V34" s="60"/>
-      <c r="W34" s="55"/>
-      <c r="X34" s="55"/>
-      <c r="Y34" s="56"/>
+      <c r="W34" s="94"/>
+      <c r="X34" s="106"/>
+      <c r="Y34" s="106"/>
       <c r="Z34" s="57"/>
       <c r="AA34" s="58"/>
-      <c r="AB34" s="55"/>
-      <c r="AC34" s="103"/>
-      <c r="AD34" s="101"/>
-      <c r="AE34" s="101"/>
-      <c r="AF34" s="101"/>
+      <c r="AB34" s="94"/>
+      <c r="AC34" s="94"/>
+      <c r="AD34" s="92"/>
+      <c r="AE34" s="92"/>
+      <c r="AF34" s="92"/>
       <c r="AG34" s="57"/>
       <c r="AH34" s="58"/>
       <c r="AI34" s="59"/>
@@ -4631,8 +4690,8 @@
       <c r="AO34" s="58"/>
       <c r="AP34" s="59"/>
       <c r="AQ34" s="60"/>
-      <c r="AR34" s="103"/>
-      <c r="AS34" s="103"/>
+      <c r="AR34" s="55"/>
+      <c r="AS34" s="55"/>
       <c r="AT34" s="55"/>
       <c r="AU34" s="57"/>
       <c r="AV34" s="58"/>
@@ -4686,9 +4745,9 @@
       <c r="AA35" s="58"/>
       <c r="AB35" s="55"/>
       <c r="AC35" s="55"/>
-      <c r="AD35" s="101"/>
-      <c r="AE35" s="101"/>
-      <c r="AF35" s="101"/>
+      <c r="AD35" s="92"/>
+      <c r="AE35" s="92"/>
+      <c r="AF35" s="92"/>
       <c r="AG35" s="57"/>
       <c r="AH35" s="58"/>
       <c r="AI35" s="68"/>
@@ -4702,7 +4761,7 @@
       <c r="AQ35" s="69"/>
       <c r="AR35" s="55"/>
       <c r="AS35" s="55"/>
-      <c r="AT35" s="56"/>
+      <c r="AT35" s="55"/>
       <c r="AU35" s="57"/>
       <c r="AV35" s="58"/>
       <c r="AW35" s="68"/>
@@ -4833,9 +4892,9 @@
       <c r="AA37" s="58"/>
       <c r="AB37" s="55"/>
       <c r="AC37" s="55"/>
-      <c r="AD37" s="101"/>
-      <c r="AE37" s="101"/>
-      <c r="AF37" s="101"/>
+      <c r="AD37" s="92"/>
+      <c r="AE37" s="92"/>
+      <c r="AF37" s="92"/>
       <c r="AG37" s="57"/>
       <c r="AH37" s="58"/>
       <c r="AI37" s="53"/>
@@ -4847,8 +4906,8 @@
       <c r="AO37" s="58"/>
       <c r="AP37" s="53"/>
       <c r="AQ37" s="54"/>
-      <c r="AR37" s="103"/>
-      <c r="AS37" s="103"/>
+      <c r="AR37" s="94"/>
+      <c r="AS37" s="94"/>
       <c r="AT37" s="56"/>
       <c r="AU37" s="57"/>
       <c r="AV37" s="58"/>
@@ -4902,9 +4961,9 @@
       <c r="AA38" s="58"/>
       <c r="AB38" s="55"/>
       <c r="AC38" s="55"/>
-      <c r="AD38" s="101"/>
-      <c r="AE38" s="101"/>
-      <c r="AF38" s="101"/>
+      <c r="AD38" s="92"/>
+      <c r="AE38" s="92"/>
+      <c r="AF38" s="92"/>
       <c r="AG38" s="57"/>
       <c r="AH38" s="58"/>
       <c r="AI38" s="68"/>
@@ -5049,9 +5108,9 @@
       <c r="AA40" s="58"/>
       <c r="AB40" s="55"/>
       <c r="AC40" s="55"/>
-      <c r="AD40" s="101"/>
-      <c r="AE40" s="101"/>
-      <c r="AF40" s="101"/>
+      <c r="AD40" s="92"/>
+      <c r="AE40" s="92"/>
+      <c r="AF40" s="92"/>
       <c r="AG40" s="57"/>
       <c r="AH40" s="58"/>
       <c r="AI40" s="53"/>
@@ -5063,7 +5122,7 @@
       <c r="AO40" s="58"/>
       <c r="AP40" s="53"/>
       <c r="AQ40" s="54"/>
-      <c r="AR40" s="55"/>
+      <c r="AR40" s="94"/>
       <c r="AS40" s="55"/>
       <c r="AT40" s="56"/>
       <c r="AU40" s="57"/>
@@ -5122,9 +5181,9 @@
       <c r="AA41" s="58"/>
       <c r="AB41" s="55"/>
       <c r="AC41" s="55"/>
-      <c r="AD41" s="101"/>
-      <c r="AE41" s="101"/>
-      <c r="AF41" s="101"/>
+      <c r="AD41" s="92"/>
+      <c r="AE41" s="92"/>
+      <c r="AF41" s="92"/>
       <c r="AG41" s="57"/>
       <c r="AH41" s="58"/>
       <c r="AI41" s="59"/>
@@ -5136,9 +5195,9 @@
       <c r="AO41" s="58"/>
       <c r="AP41" s="59"/>
       <c r="AQ41" s="60"/>
-      <c r="AR41" s="55"/>
-      <c r="AS41" s="103"/>
-      <c r="AT41" s="56"/>
+      <c r="AR41" s="94"/>
+      <c r="AS41" s="55"/>
+      <c r="AT41" s="55"/>
       <c r="AU41" s="57"/>
       <c r="AV41" s="58"/>
       <c r="AW41" s="59"/>
@@ -5191,9 +5250,9 @@
       <c r="AA42" s="58"/>
       <c r="AB42" s="55"/>
       <c r="AC42" s="55"/>
-      <c r="AD42" s="101"/>
-      <c r="AE42" s="101"/>
-      <c r="AF42" s="101"/>
+      <c r="AD42" s="92"/>
+      <c r="AE42" s="92"/>
+      <c r="AF42" s="92"/>
       <c r="AG42" s="57"/>
       <c r="AH42" s="58"/>
       <c r="AI42" s="68"/>
@@ -5207,7 +5266,7 @@
       <c r="AQ42" s="69"/>
       <c r="AR42" s="55"/>
       <c r="AS42" s="55"/>
-      <c r="AT42" s="56"/>
+      <c r="AT42" s="55"/>
       <c r="AU42" s="57"/>
       <c r="AV42" s="58"/>
       <c r="AW42" s="68"/>
@@ -5232,11 +5291,11 @@
       </c>
       <c r="C43" s="37">
         <f>C39+C36+C31+C18+C14+C9</f>
-        <v>82.5</v>
+        <v>88.800000000000011</v>
       </c>
       <c r="D43" s="37">
         <f>D39+D36+D31+D18+D14+D9</f>
-        <v>4.16</v>
+        <v>6.32</v>
       </c>
       <c r="E43" s="37"/>
       <c r="F43" s="38"/>
@@ -5254,7 +5313,7 @@
       </c>
       <c r="J43" s="39">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>6.16</v>
       </c>
       <c r="K43" s="39">
         <f t="shared" si="3"/>
@@ -5511,10 +5570,10 @@
   <sheetData>
     <row r="1" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="99" t="s">
+      <c r="A2" s="104" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="100"/>
+      <c r="B2" s="105"/>
       <c r="C2" s="78" t="s">
         <v>14</v>
       </c>
@@ -5523,48 +5582,48 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="97" t="str">
+      <c r="A3" s="102" t="str">
         <f>Zeitplanung!B9</f>
         <v>Administration, Planung</v>
       </c>
-      <c r="B3" s="98"/>
+      <c r="B3" s="103"/>
       <c r="C3" s="79">
         <f>Zeitplanung!C9</f>
         <v>4.5</v>
       </c>
       <c r="D3" s="79">
         <f>Zeitplanung!D9</f>
-        <v>4.16</v>
+        <v>2.3199999999999998</v>
       </c>
       <c r="E3" s="81"/>
       <c r="F3" s="80"/>
     </row>
     <row r="4" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="97" t="str">
+      <c r="A4" s="102" t="str">
         <f>Zeitplanung!B14</f>
         <v>Analyse &amp; Design</v>
       </c>
-      <c r="B4" s="98"/>
+      <c r="B4" s="103"/>
       <c r="C4" s="79">
         <f>Zeitplanung!C14</f>
         <v>7</v>
       </c>
       <c r="D4" s="79">
         <f>Zeitplanung!D14</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E4" s="81"/>
       <c r="F4" s="80"/>
     </row>
     <row r="5" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="97" t="str">
+      <c r="A5" s="102" t="str">
         <f>Zeitplanung!B18</f>
         <v>Implementation</v>
       </c>
-      <c r="B5" s="98"/>
+      <c r="B5" s="103"/>
       <c r="C5" s="79">
         <f>Zeitplanung!C18</f>
-        <v>54.5</v>
+        <v>60.800000000000011</v>
       </c>
       <c r="D5" s="79">
         <f>Zeitplanung!D18</f>
@@ -5574,11 +5633,11 @@
       <c r="F5" s="80"/>
     </row>
     <row r="6" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="97" t="str">
+      <c r="A6" s="102" t="str">
         <f>Zeitplanung!B31</f>
         <v>Testen</v>
       </c>
-      <c r="B6" s="98"/>
+      <c r="B6" s="103"/>
       <c r="C6" s="79">
         <f>Zeitplanung!C31</f>
         <v>8.5</v>
@@ -5590,11 +5649,11 @@
       <c r="F6" s="80"/>
     </row>
     <row r="7" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="97" t="str">
+      <c r="A7" s="102" t="str">
         <f>Zeitplanung!B36</f>
         <v>Diverses</v>
       </c>
-      <c r="B7" s="98"/>
+      <c r="B7" s="103"/>
       <c r="C7" s="79">
         <f>Zeitplanung!C36</f>
         <v>4</v>
@@ -5606,11 +5665,11 @@
       <c r="F7" s="80"/>
     </row>
     <row r="8" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="97" t="str">
+      <c r="A8" s="102" t="str">
         <f>Zeitplanung!B39</f>
         <v>Abschluss</v>
       </c>
-      <c r="B8" s="98"/>
+      <c r="B8" s="103"/>
       <c r="C8" s="79">
         <f>Zeitplanung!C39</f>
         <v>4</v>

</xml_diff>

<commit_message>
assets folder, Zeitplan, Button
</commit_message>
<xml_diff>
--- a/docs/Zeitplanung.xlsx
+++ b/docs/Zeitplanung.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/natascha/Desktop/Memory-Collector/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39061389-E65D-234E-8B3C-39884144E51F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{145A9FDC-0A77-5C42-99C1-1E1B370F434B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="35840" yWindow="-8820" windowWidth="38400" windowHeight="21140" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20400" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zeitplanung" sheetId="1" r:id="rId1"/>
@@ -269,7 +269,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <name val="Times New Roman"/>
@@ -373,6 +373,12 @@
       <name val="Segoe UI"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="19">
@@ -1126,7 +1132,7 @@
     </xf>
     <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1455,6 +1461,16 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1486,13 +1502,7 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1673,10 +1683,10 @@
                   <c:v>2.3199999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2183,8 +2193,8 @@
   </sheetPr>
   <dimension ref="A1:BJ43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="X35" sqref="X35"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2503,88 +2513,88 @@
     <row r="7" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9"/>
       <c r="B7" s="27"/>
-      <c r="C7" s="97" t="s">
+      <c r="C7" s="100" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="97"/>
+      <c r="D7" s="100"/>
       <c r="E7" s="28" t="s">
         <v>20</v>
       </c>
       <c r="F7" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="98" t="s">
+      <c r="G7" s="101" t="s">
         <v>32</v>
       </c>
-      <c r="H7" s="98"/>
-      <c r="I7" s="98"/>
-      <c r="J7" s="98"/>
-      <c r="K7" s="98"/>
-      <c r="L7" s="98"/>
-      <c r="M7" s="99"/>
-      <c r="N7" s="98" t="s">
+      <c r="H7" s="101"/>
+      <c r="I7" s="101"/>
+      <c r="J7" s="101"/>
+      <c r="K7" s="101"/>
+      <c r="L7" s="101"/>
+      <c r="M7" s="102"/>
+      <c r="N7" s="101" t="s">
         <v>33</v>
       </c>
-      <c r="O7" s="98"/>
-      <c r="P7" s="98"/>
-      <c r="Q7" s="98"/>
-      <c r="R7" s="98"/>
-      <c r="S7" s="98"/>
-      <c r="T7" s="99"/>
-      <c r="U7" s="98" t="s">
+      <c r="O7" s="101"/>
+      <c r="P7" s="101"/>
+      <c r="Q7" s="101"/>
+      <c r="R7" s="101"/>
+      <c r="S7" s="101"/>
+      <c r="T7" s="102"/>
+      <c r="U7" s="101" t="s">
         <v>34</v>
       </c>
-      <c r="V7" s="98"/>
-      <c r="W7" s="98"/>
-      <c r="X7" s="98"/>
-      <c r="Y7" s="98"/>
-      <c r="Z7" s="98"/>
-      <c r="AA7" s="99"/>
-      <c r="AB7" s="100" t="s">
+      <c r="V7" s="101"/>
+      <c r="W7" s="101"/>
+      <c r="X7" s="101"/>
+      <c r="Y7" s="101"/>
+      <c r="Z7" s="101"/>
+      <c r="AA7" s="102"/>
+      <c r="AB7" s="103" t="s">
         <v>35</v>
       </c>
-      <c r="AC7" s="98"/>
-      <c r="AD7" s="98"/>
-      <c r="AE7" s="98"/>
-      <c r="AF7" s="98"/>
-      <c r="AG7" s="98"/>
-      <c r="AH7" s="99"/>
-      <c r="AI7" s="98" t="s">
+      <c r="AC7" s="101"/>
+      <c r="AD7" s="101"/>
+      <c r="AE7" s="101"/>
+      <c r="AF7" s="101"/>
+      <c r="AG7" s="101"/>
+      <c r="AH7" s="102"/>
+      <c r="AI7" s="101" t="s">
         <v>50</v>
       </c>
-      <c r="AJ7" s="98"/>
-      <c r="AK7" s="98"/>
-      <c r="AL7" s="98"/>
-      <c r="AM7" s="98"/>
-      <c r="AN7" s="98"/>
-      <c r="AO7" s="99"/>
-      <c r="AP7" s="100" t="s">
+      <c r="AJ7" s="101"/>
+      <c r="AK7" s="101"/>
+      <c r="AL7" s="101"/>
+      <c r="AM7" s="101"/>
+      <c r="AN7" s="101"/>
+      <c r="AO7" s="102"/>
+      <c r="AP7" s="103" t="s">
         <v>36</v>
       </c>
-      <c r="AQ7" s="98"/>
-      <c r="AR7" s="98"/>
-      <c r="AS7" s="98"/>
-      <c r="AT7" s="98"/>
-      <c r="AU7" s="98"/>
-      <c r="AV7" s="99"/>
-      <c r="AW7" s="98" t="s">
+      <c r="AQ7" s="101"/>
+      <c r="AR7" s="101"/>
+      <c r="AS7" s="101"/>
+      <c r="AT7" s="101"/>
+      <c r="AU7" s="101"/>
+      <c r="AV7" s="102"/>
+      <c r="AW7" s="101" t="s">
         <v>37</v>
       </c>
-      <c r="AX7" s="98"/>
-      <c r="AY7" s="98"/>
-      <c r="AZ7" s="98"/>
-      <c r="BA7" s="98"/>
-      <c r="BB7" s="98"/>
-      <c r="BC7" s="99"/>
-      <c r="BD7" s="100" t="s">
+      <c r="AX7" s="101"/>
+      <c r="AY7" s="101"/>
+      <c r="AZ7" s="101"/>
+      <c r="BA7" s="101"/>
+      <c r="BB7" s="101"/>
+      <c r="BC7" s="102"/>
+      <c r="BD7" s="103" t="s">
         <v>38</v>
       </c>
-      <c r="BE7" s="98"/>
-      <c r="BF7" s="98"/>
-      <c r="BG7" s="98"/>
-      <c r="BH7" s="98"/>
-      <c r="BI7" s="98"/>
-      <c r="BJ7" s="101"/>
+      <c r="BE7" s="101"/>
+      <c r="BF7" s="101"/>
+      <c r="BG7" s="101"/>
+      <c r="BH7" s="101"/>
+      <c r="BI7" s="101"/>
+      <c r="BJ7" s="104"/>
     </row>
     <row r="8" spans="1:62" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
@@ -3167,7 +3177,7 @@
       </c>
       <c r="D14" s="42">
         <f>SUM(D15:D17)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E14" s="32"/>
       <c r="F14" s="31"/>
@@ -3317,7 +3327,7 @@
       </c>
       <c r="D16" s="82">
         <f>SUM(G16:BJ16)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E16" s="50"/>
       <c r="F16" s="51"/>
@@ -3325,7 +3335,9 @@
       <c r="H16" s="60"/>
       <c r="I16" s="55"/>
       <c r="J16" s="55"/>
-      <c r="K16" s="56"/>
+      <c r="K16" s="109">
+        <v>2</v>
+      </c>
       <c r="L16" s="57"/>
       <c r="M16" s="58"/>
       <c r="N16" s="59"/>
@@ -3460,7 +3472,7 @@
       </c>
       <c r="D18" s="42">
         <f>SUM(D19:D30)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E18" s="32"/>
       <c r="F18" s="31"/>
@@ -3606,7 +3618,7 @@
       </c>
       <c r="D20" s="82">
         <f t="shared" ref="D20:D30" si="0">SUM(G20:BJ20)</f>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="E20" s="50"/>
       <c r="F20" s="51"/>
@@ -3614,13 +3626,15 @@
       <c r="H20" s="60"/>
       <c r="I20" s="55"/>
       <c r="J20" s="55"/>
-      <c r="K20" s="96"/>
+      <c r="K20" s="96">
+        <v>2.5</v>
+      </c>
       <c r="L20" s="57"/>
       <c r="M20" s="58"/>
       <c r="N20" s="59"/>
       <c r="O20" s="60"/>
       <c r="P20" s="94"/>
-      <c r="Q20" s="107"/>
+      <c r="Q20" s="98"/>
       <c r="R20" s="55"/>
       <c r="S20" s="57"/>
       <c r="T20" s="58"/>
@@ -3679,7 +3693,7 @@
       </c>
       <c r="D21" s="82">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="E21" s="50">
         <v>1</v>
@@ -3689,7 +3703,9 @@
       <c r="H21" s="60"/>
       <c r="I21" s="55"/>
       <c r="J21" s="55"/>
-      <c r="K21" s="63"/>
+      <c r="K21" s="63">
+        <v>2.5</v>
+      </c>
       <c r="L21" s="57"/>
       <c r="M21" s="58"/>
       <c r="N21" s="59"/>
@@ -3926,7 +3942,7 @@
       <c r="T24" s="58"/>
       <c r="U24" s="59"/>
       <c r="V24" s="60"/>
-      <c r="W24" s="108"/>
+      <c r="W24" s="99"/>
       <c r="X24" s="55"/>
       <c r="Y24" s="55"/>
       <c r="Z24" s="57"/>
@@ -4438,7 +4454,7 @@
       <c r="H31" s="73"/>
       <c r="I31" s="73"/>
       <c r="J31" s="73"/>
-      <c r="K31" s="74"/>
+      <c r="K31" s="56"/>
       <c r="L31" s="74"/>
       <c r="M31" s="75"/>
       <c r="N31" s="72"/>
@@ -4670,8 +4686,8 @@
       <c r="U34" s="59"/>
       <c r="V34" s="60"/>
       <c r="W34" s="94"/>
-      <c r="X34" s="106"/>
-      <c r="Y34" s="106"/>
+      <c r="X34" s="97"/>
+      <c r="Y34" s="97"/>
       <c r="Z34" s="57"/>
       <c r="AA34" s="58"/>
       <c r="AB34" s="94"/>
@@ -5295,7 +5311,7 @@
       </c>
       <c r="D43" s="37">
         <f>D39+D36+D31+D18+D14+D9</f>
-        <v>6.32</v>
+        <v>13.32</v>
       </c>
       <c r="E43" s="37"/>
       <c r="F43" s="38"/>
@@ -5317,7 +5333,7 @@
       </c>
       <c r="K43" s="39">
         <f t="shared" si="3"/>
-        <v>0.16</v>
+        <v>7.16</v>
       </c>
       <c r="L43" s="39">
         <f t="shared" si="3"/>
@@ -5570,10 +5586,10 @@
   <sheetData>
     <row r="1" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="104" t="s">
+      <c r="A2" s="107" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="105"/>
+      <c r="B2" s="108"/>
       <c r="C2" s="78" t="s">
         <v>14</v>
       </c>
@@ -5582,11 +5598,11 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="102" t="str">
+      <c r="A3" s="105" t="str">
         <f>Zeitplanung!B9</f>
         <v>Administration, Planung</v>
       </c>
-      <c r="B3" s="103"/>
+      <c r="B3" s="106"/>
       <c r="C3" s="79">
         <f>Zeitplanung!C9</f>
         <v>4.5</v>
@@ -5599,45 +5615,45 @@
       <c r="F3" s="80"/>
     </row>
     <row r="4" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="102" t="str">
+      <c r="A4" s="105" t="str">
         <f>Zeitplanung!B14</f>
         <v>Analyse &amp; Design</v>
       </c>
-      <c r="B4" s="103"/>
+      <c r="B4" s="106"/>
       <c r="C4" s="79">
         <f>Zeitplanung!C14</f>
         <v>7</v>
       </c>
       <c r="D4" s="79">
         <f>Zeitplanung!D14</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E4" s="81"/>
       <c r="F4" s="80"/>
     </row>
     <row r="5" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="102" t="str">
+      <c r="A5" s="105" t="str">
         <f>Zeitplanung!B18</f>
         <v>Implementation</v>
       </c>
-      <c r="B5" s="103"/>
+      <c r="B5" s="106"/>
       <c r="C5" s="79">
         <f>Zeitplanung!C18</f>
         <v>60.800000000000011</v>
       </c>
       <c r="D5" s="79">
         <f>Zeitplanung!D18</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E5" s="81"/>
       <c r="F5" s="80"/>
     </row>
     <row r="6" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="102" t="str">
+      <c r="A6" s="105" t="str">
         <f>Zeitplanung!B31</f>
         <v>Testen</v>
       </c>
-      <c r="B6" s="103"/>
+      <c r="B6" s="106"/>
       <c r="C6" s="79">
         <f>Zeitplanung!C31</f>
         <v>8.5</v>
@@ -5649,11 +5665,11 @@
       <c r="F6" s="80"/>
     </row>
     <row r="7" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="102" t="str">
+      <c r="A7" s="105" t="str">
         <f>Zeitplanung!B36</f>
         <v>Diverses</v>
       </c>
-      <c r="B7" s="103"/>
+      <c r="B7" s="106"/>
       <c r="C7" s="79">
         <f>Zeitplanung!C36</f>
         <v>4</v>
@@ -5665,11 +5681,11 @@
       <c r="F7" s="80"/>
     </row>
     <row r="8" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="102" t="str">
+      <c r="A8" s="105" t="str">
         <f>Zeitplanung!B39</f>
         <v>Abschluss</v>
       </c>
-      <c r="B8" s="103"/>
+      <c r="B8" s="106"/>
       <c r="C8" s="79">
         <f>Zeitplanung!C39</f>
         <v>4</v>

</xml_diff>